<commit_message>
Updated with connectors and through holes
</commit_message>
<xml_diff>
--- a/MotorDriverBreakout/MotorDriverBreakoutComponents.xlsx
+++ b/MotorDriverBreakout/MotorDriverBreakoutComponents.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11214"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elvy/Documents/Trellis/in-pipe-electronics-software/MotorDriverBreakout/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BCD7651E-F221-8A49-AE42-535BA048E219}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CED92B58-7612-0247-A7C0-ABE320942A80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-51200" yWindow="-9060" windowWidth="51200" windowHeight="28180" xr2:uid="{1072E8A8-AAA4-AA45-98F8-2595D94DABE6}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="29400" windowHeight="18440" xr2:uid="{1072E8A8-AAA4-AA45-98F8-2595D94DABE6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t>Component</t>
   </si>
@@ -123,6 +123,21 @@
   </si>
   <si>
     <t>https://www.ti.com/lit/ds/symlink/tpsm33625.pdf</t>
+  </si>
+  <si>
+    <t>JST SH 4 position 1 mm pitch connector</t>
+  </si>
+  <si>
+    <t>1528-4208-ND</t>
+  </si>
+  <si>
+    <t>This might be a 10 pack (listed on Adafruit, but not sure)</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/adafruit-industries-llc/4208/10230005</t>
+  </si>
+  <si>
+    <t>https://cdn-shop.adafruit.com/product-files/4208/4208_Kaweei_C13396_diagram.pdf</t>
   </si>
 </sst>
 </file>
@@ -505,10 +520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5D6324C-B691-594D-AFA2-B412E6A3CB5D}">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -584,7 +599,7 @@
         <v>1.27</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D6" si="0">B3*C3</f>
+        <f t="shared" ref="D3:D7" si="0">B3*C3</f>
         <v>2.54</v>
       </c>
       <c r="E3" t="s">
@@ -673,6 +688,33 @@
       </c>
       <c r="H6" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>3.95</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>7.9</v>
+      </c>
+      <c r="E7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>